<commit_message>
Fixed the question generator controller
</commit_message>
<xml_diff>
--- a/uploads/Question 01-50.xlsx
+++ b/uploads/Question 01-50.xlsx
@@ -2180,7 +2180,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" ht="16.5">
+    <row r="8" ht="16.199999999999999">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" ht="33">
+    <row r="9" ht="32.399999999999999">
       <c r="A9" s="8">
         <v>2</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" ht="16.5">
+    <row r="10" ht="16.199999999999999">
       <c r="A10" s="15">
         <v>3</v>
       </c>
@@ -2306,7 +2306,7 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
     </row>
-    <row r="11" ht="16.5">
+    <row r="11" ht="16.199999999999999">
       <c r="A11" s="17">
         <v>4</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
     </row>
-    <row r="12" ht="49.5">
+    <row r="12" ht="48.600000000000001">
       <c r="A12" s="17">
         <v>5</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
     </row>
-    <row r="13" ht="33">
+    <row r="13" ht="32.399999999999999">
       <c r="A13" s="17">
         <v>6</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
     </row>
-    <row r="14" ht="49.5">
+    <row r="14" ht="48.600000000000001">
       <c r="A14" s="17">
         <v>7</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
     </row>
-    <row r="15" ht="16.5">
+    <row r="15" ht="16.199999999999999">
       <c r="A15" s="17">
         <v>8</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
     </row>
-    <row r="16" ht="16.5">
+    <row r="16" ht="16.199999999999999">
       <c r="A16" s="17">
         <v>9</v>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
     </row>
-    <row r="17" ht="49.5">
+    <row r="17" ht="48.600000000000001">
       <c r="A17" s="17">
         <v>10</v>
       </c>
@@ -2600,7 +2600,7 @@
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
     </row>
-    <row r="18" ht="33">
+    <row r="18" ht="32.399999999999999">
       <c r="A18" s="17">
         <v>11</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
     </row>
-    <row r="19" ht="49.5">
+    <row r="19" ht="48.600000000000001">
       <c r="A19" s="17">
         <v>12</v>
       </c>
@@ -2682,7 +2682,7 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" ht="33">
+    <row r="20" ht="32.399999999999999">
       <c r="A20" s="17">
         <v>13</v>
       </c>
@@ -2808,7 +2808,7 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
     </row>
-    <row r="23" ht="27">
+    <row r="23" ht="26.399999999999999">
       <c r="A23" s="23">
         <v>16</v>
       </c>
@@ -2976,7 +2976,7 @@
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
     </row>
-    <row r="27" ht="27">
+    <row r="27" ht="26.399999999999999">
       <c r="A27" s="23">
         <v>20</v>
       </c>
@@ -3692,7 +3692,7 @@
       <c r="Y43" s="12"/>
       <c r="Z43" s="12"/>
     </row>
-    <row r="44" ht="40.5">
+    <row r="44" ht="39.600000000000001">
       <c r="A44" s="23">
         <v>37</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="Y44" s="12"/>
       <c r="Z44" s="12"/>
     </row>
-    <row r="45" ht="27">
+    <row r="45" ht="26.399999999999999">
       <c r="A45" s="23">
         <v>38</v>
       </c>
@@ -3776,7 +3776,7 @@
       <c r="Y45" s="12"/>
       <c r="Z45" s="12"/>
     </row>
-    <row r="46" ht="40.5">
+    <row r="46" ht="39.600000000000001">
       <c r="A46" s="23">
         <v>39</v>
       </c>
@@ -3860,7 +3860,7 @@
       <c r="Y47" s="12"/>
       <c r="Z47" s="12"/>
     </row>
-    <row r="48" ht="27">
+    <row r="48" ht="26.399999999999999">
       <c r="A48" s="23">
         <v>41</v>
       </c>
@@ -3944,7 +3944,7 @@
       <c r="Y49" s="12"/>
       <c r="Z49" s="12"/>
     </row>
-    <row r="50" ht="27">
+    <row r="50" ht="26.399999999999999">
       <c r="A50" s="23">
         <v>43</v>
       </c>
@@ -3986,7 +3986,7 @@
       <c r="Y50" s="12"/>
       <c r="Z50" s="12"/>
     </row>
-    <row r="51" ht="27">
+    <row r="51" ht="26.399999999999999">
       <c r="A51" s="23">
         <v>44</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
     </row>
-    <row r="53" ht="27">
+    <row r="53" ht="26.399999999999999">
       <c r="A53" s="23">
         <v>46</v>
       </c>
@@ -4112,7 +4112,7 @@
       <c r="Y53" s="12"/>
       <c r="Z53" s="12"/>
     </row>
-    <row r="54" ht="27">
+    <row r="54" ht="26.399999999999999">
       <c r="A54" s="23">
         <v>47</v>
       </c>
@@ -4154,7 +4154,7 @@
       <c r="Y54" s="12"/>
       <c r="Z54" s="12"/>
     </row>
-    <row r="55" ht="27">
+    <row r="55" ht="26.399999999999999">
       <c r="A55" s="23">
         <v>48</v>
       </c>
@@ -4196,7 +4196,7 @@
       <c r="Y55" s="12"/>
       <c r="Z55" s="12"/>
     </row>
-    <row r="56" ht="27">
+    <row r="56" ht="26.399999999999999">
       <c r="A56" s="23">
         <v>49</v>
       </c>
@@ -4238,7 +4238,7 @@
       <c r="Y56" s="12"/>
       <c r="Z56" s="12"/>
     </row>
-    <row r="57" ht="27">
+    <row r="57" ht="26.399999999999999">
       <c r="A57" s="23">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
changed the UI of client side
</commit_message>
<xml_diff>
--- a/uploads/Question 01-50.xlsx
+++ b/uploads/Question 01-50.xlsx
@@ -2180,7 +2180,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" ht="16.199999999999999">
+    <row r="8" ht="16.5">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" ht="32.399999999999999">
+    <row r="9" ht="33">
       <c r="A9" s="8">
         <v>2</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" ht="16.199999999999999">
+    <row r="10" ht="16.5">
       <c r="A10" s="15">
         <v>3</v>
       </c>
@@ -2306,7 +2306,7 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
     </row>
-    <row r="11" ht="16.199999999999999">
+    <row r="11" ht="16.5">
       <c r="A11" s="17">
         <v>4</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
     </row>
-    <row r="12" ht="48.600000000000001">
+    <row r="12" ht="49.5">
       <c r="A12" s="17">
         <v>5</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
     </row>
-    <row r="13" ht="32.399999999999999">
+    <row r="13" ht="33">
       <c r="A13" s="17">
         <v>6</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
     </row>
-    <row r="14" ht="48.600000000000001">
+    <row r="14" ht="49.5">
       <c r="A14" s="17">
         <v>7</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
     </row>
-    <row r="15" ht="16.199999999999999">
+    <row r="15" ht="16.5">
       <c r="A15" s="17">
         <v>8</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
     </row>
-    <row r="16" ht="16.199999999999999">
+    <row r="16" ht="16.5">
       <c r="A16" s="17">
         <v>9</v>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
     </row>
-    <row r="17" ht="48.600000000000001">
+    <row r="17" ht="49.5">
       <c r="A17" s="17">
         <v>10</v>
       </c>
@@ -2600,7 +2600,7 @@
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
     </row>
-    <row r="18" ht="32.399999999999999">
+    <row r="18" ht="33">
       <c r="A18" s="17">
         <v>11</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
     </row>
-    <row r="19" ht="48.600000000000001">
+    <row r="19" ht="49.5">
       <c r="A19" s="17">
         <v>12</v>
       </c>
@@ -2682,7 +2682,7 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" ht="32.399999999999999">
+    <row r="20" ht="33">
       <c r="A20" s="17">
         <v>13</v>
       </c>
@@ -2808,7 +2808,7 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
     </row>
-    <row r="23" ht="26.399999999999999">
+    <row r="23" ht="27">
       <c r="A23" s="23">
         <v>16</v>
       </c>
@@ -2976,7 +2976,7 @@
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
     </row>
-    <row r="27" ht="26.399999999999999">
+    <row r="27" ht="27">
       <c r="A27" s="23">
         <v>20</v>
       </c>
@@ -3692,7 +3692,7 @@
       <c r="Y43" s="12"/>
       <c r="Z43" s="12"/>
     </row>
-    <row r="44" ht="39.600000000000001">
+    <row r="44" ht="40.5">
       <c r="A44" s="23">
         <v>37</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="Y44" s="12"/>
       <c r="Z44" s="12"/>
     </row>
-    <row r="45" ht="26.399999999999999">
+    <row r="45" ht="27">
       <c r="A45" s="23">
         <v>38</v>
       </c>
@@ -3776,7 +3776,7 @@
       <c r="Y45" s="12"/>
       <c r="Z45" s="12"/>
     </row>
-    <row r="46" ht="39.600000000000001">
+    <row r="46" ht="40.5">
       <c r="A46" s="23">
         <v>39</v>
       </c>
@@ -3860,7 +3860,7 @@
       <c r="Y47" s="12"/>
       <c r="Z47" s="12"/>
     </row>
-    <row r="48" ht="26.399999999999999">
+    <row r="48" ht="27">
       <c r="A48" s="23">
         <v>41</v>
       </c>
@@ -3944,7 +3944,7 @@
       <c r="Y49" s="12"/>
       <c r="Z49" s="12"/>
     </row>
-    <row r="50" ht="26.399999999999999">
+    <row r="50" ht="27">
       <c r="A50" s="23">
         <v>43</v>
       </c>
@@ -3986,7 +3986,7 @@
       <c r="Y50" s="12"/>
       <c r="Z50" s="12"/>
     </row>
-    <row r="51" ht="26.399999999999999">
+    <row r="51" ht="27">
       <c r="A51" s="23">
         <v>44</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
     </row>
-    <row r="53" ht="26.399999999999999">
+    <row r="53" ht="27">
       <c r="A53" s="23">
         <v>46</v>
       </c>
@@ -4112,7 +4112,7 @@
       <c r="Y53" s="12"/>
       <c r="Z53" s="12"/>
     </row>
-    <row r="54" ht="26.399999999999999">
+    <row r="54" ht="27">
       <c r="A54" s="23">
         <v>47</v>
       </c>
@@ -4154,7 +4154,7 @@
       <c r="Y54" s="12"/>
       <c r="Z54" s="12"/>
     </row>
-    <row r="55" ht="26.399999999999999">
+    <row r="55" ht="27">
       <c r="A55" s="23">
         <v>48</v>
       </c>
@@ -4196,7 +4196,7 @@
       <c r="Y55" s="12"/>
       <c r="Z55" s="12"/>
     </row>
-    <row r="56" ht="26.399999999999999">
+    <row r="56" ht="27">
       <c r="A56" s="23">
         <v>49</v>
       </c>
@@ -4238,7 +4238,7 @@
       <c r="Y56" s="12"/>
       <c r="Z56" s="12"/>
     </row>
-    <row r="57" ht="26.399999999999999">
+    <row r="57" ht="27">
       <c r="A57" s="23">
         <v>50</v>
       </c>

</xml_diff>